<commit_message>
Update easy upload template to include variables
</commit_message>
<xml_diff>
--- a/public/files/templates/easy-upload.xlsx
+++ b/public/files/templates/easy-upload.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/apps/cost-control/public/files/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/code/cost-control/public/files/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E1CBA8-1FD2-9C46-94D3-CC053CB07355}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2180" windowWidth="24160" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="1440" yWindow="2180" windowWidth="24160" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" calcMode="manual" concurrentCalc="0"/>
+  <calcPr calcId="150000" calcMode="manual"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>WBS Code</t>
   </si>
@@ -36,12 +37,36 @@
   </si>
   <si>
     <t>Cost Account</t>
+  </si>
+  <si>
+    <t>$v1</t>
+  </si>
+  <si>
+    <t>$v2</t>
+  </si>
+  <si>
+    <t>$v3</t>
+  </si>
+  <si>
+    <t>$v4</t>
+  </si>
+  <si>
+    <t>$v5</t>
+  </si>
+  <si>
+    <t>$v6</t>
+  </si>
+  <si>
+    <t>$v7</t>
+  </si>
+  <si>
+    <t>$v8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -83,17 +108,28 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:C2"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="WBS Code"/>
-    <tableColumn id="2" name="Breakdown Template Code"/>
-    <tableColumn id="3" name="Cost Account"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:K2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="WBS Code"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Breakdown Template Code"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Cost Account"/>
+    <tableColumn id="4" xr3:uid="{8BE52C18-8A2E-EB4C-A3F7-4F335302E40F}" name="$v1"/>
+    <tableColumn id="5" xr3:uid="{A4E047E2-7680-DB42-BFDD-2CEF40D0B09E}" name="$v2"/>
+    <tableColumn id="6" xr3:uid="{CB1606A1-32DF-DA41-BBEA-CE949CB7A340}" name="$v3"/>
+    <tableColumn id="7" xr3:uid="{F1771351-B159-4742-88F4-C6B8A4937882}" name="$v4"/>
+    <tableColumn id="8" xr3:uid="{588B0B28-3165-9E41-9F58-877A7CE269DC}" name="$v5"/>
+    <tableColumn id="9" xr3:uid="{65102C95-32A7-CB4D-8974-541B7A4A9A01}" name="$v6"/>
+    <tableColumn id="10" xr3:uid="{E169FE1D-816A-A441-B751-F96F081D5153}" name="$v7"/>
+    <tableColumn id="11" xr3:uid="{8D9ABDFA-421D-0940-A256-55D8DB960031}" name="$v8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -361,8 +397,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -375,7 +411,7 @@
     <col min="3" max="3" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -384,6 +420,30 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>